<commit_message>
refactor nda and probtree
</commit_message>
<xml_diff>
--- a/examples/game_of_24/output/optimized_validation/dataset_measurement.xlsx
+++ b/examples/game_of_24/output/optimized_validation/dataset_measurement.xlsx
@@ -53,7 +53,7 @@
     <t>success</t>
   </si>
   <si>
-    <t>&lt;function mean at 0x1072640e0&gt;</t>
+    <t>&lt;function mean at 0x1028cc0e0&gt;</t>
   </si>
   <si>
     <t>min_runs</t>
@@ -475,7 +475,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>192.9722907543182</v>
+        <v>249.0911111831665</v>
       </c>
     </row>
   </sheetData>
@@ -579,10 +579,10 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.62</v>
+        <v>0.66</v>
       </c>
       <c r="C2">
-        <v>0.1935927981119528</v>
+        <v>0.1889352446120098</v>
       </c>
     </row>
   </sheetData>
@@ -638,28 +638,28 @@
         <v>26</v>
       </c>
       <c r="C2">
-        <v>68676.17</v>
+        <v>68304.25</v>
       </c>
       <c r="D2">
-        <v>8157.47</v>
+        <v>8094.95</v>
       </c>
       <c r="E2">
-        <v>76833.64</v>
+        <v>76399.2</v>
       </c>
       <c r="F2">
-        <v>0.1716904250000003</v>
+        <v>0.1707606250000003</v>
       </c>
       <c r="G2">
-        <v>0.08157470000000032</v>
+        <v>0.08094950000000029</v>
       </c>
       <c r="H2">
-        <v>0.2532651249999999</v>
+        <v>0.251710125</v>
       </c>
       <c r="I2">
-        <v>427.0683864096203</v>
+        <v>451.6684336052323</v>
       </c>
       <c r="J2">
-        <v>194.71</v>
+        <v>193.36</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -670,28 +670,28 @@
         <v>27</v>
       </c>
       <c r="C3">
-        <v>53378.99</v>
+        <v>54965.63</v>
       </c>
       <c r="D3">
-        <v>6197.75</v>
+        <v>6344.98</v>
       </c>
       <c r="E3">
-        <v>59576.74</v>
+        <v>61310.61</v>
       </c>
       <c r="F3">
-        <v>0.1334474750000001</v>
+        <v>0.1374140750000001</v>
       </c>
       <c r="G3">
-        <v>0.06197750000000012</v>
+        <v>0.06344980000000014</v>
       </c>
       <c r="H3">
-        <v>0.1954249749999998</v>
+        <v>0.2008638749999999</v>
       </c>
       <c r="I3">
-        <v>328.543018137482</v>
+        <v>346.439341333895</v>
       </c>
       <c r="J3">
-        <v>153.24</v>
+        <v>157.6</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -702,28 +702,28 @@
         <v>28</v>
       </c>
       <c r="C4">
-        <v>32205.06</v>
+        <v>35291.78</v>
       </c>
       <c r="D4">
-        <v>3121.32</v>
+        <v>3485.22</v>
       </c>
       <c r="E4">
-        <v>35326.38</v>
+        <v>38777</v>
       </c>
       <c r="F4">
-        <v>0.08051265000000005</v>
+        <v>0.08822945000000008</v>
       </c>
       <c r="G4">
-        <v>0.03121319999999997</v>
+        <v>0.03485219999999999</v>
       </c>
       <c r="H4">
-        <v>0.11172585</v>
+        <v>0.12308165</v>
       </c>
       <c r="I4">
-        <v>202.5863611371885</v>
+        <v>195.0147495482466</v>
       </c>
       <c r="J4">
-        <v>95.97</v>
+        <v>104.37</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -734,25 +734,25 @@
         <v>26</v>
       </c>
       <c r="C5">
-        <v>68676.17</v>
+        <v>68304.25</v>
       </c>
       <c r="D5">
-        <v>8157.47</v>
+        <v>8094.95</v>
       </c>
       <c r="E5">
-        <v>76833.64</v>
+        <v>76399.2</v>
       </c>
       <c r="F5">
-        <v>0.1716904250000003</v>
+        <v>0.1707606250000003</v>
       </c>
       <c r="G5">
-        <v>0.08157470000000032</v>
+        <v>0.08094950000000029</v>
       </c>
       <c r="H5">
-        <v>0.2532651249999999</v>
+        <v>0.251710125</v>
       </c>
       <c r="I5">
-        <v>32.18039707909571</v>
+        <v>26.66536554811988</v>
       </c>
       <c r="J5">
         <v>6</v>
@@ -766,28 +766,28 @@
         <v>27</v>
       </c>
       <c r="C6">
-        <v>53378.99</v>
+        <v>54965.63</v>
       </c>
       <c r="D6">
-        <v>6197.75</v>
+        <v>6344.98</v>
       </c>
       <c r="E6">
-        <v>59576.74</v>
+        <v>61310.61</v>
       </c>
       <c r="F6">
-        <v>0.1334474750000001</v>
+        <v>0.1374140750000001</v>
       </c>
       <c r="G6">
-        <v>0.06197750000000012</v>
+        <v>0.06344980000000014</v>
       </c>
       <c r="H6">
-        <v>0.1954249749999998</v>
+        <v>0.2008638749999999</v>
       </c>
       <c r="I6">
-        <v>31.35769980035722</v>
+        <v>26.07851395401056</v>
       </c>
       <c r="J6">
-        <v>5.98</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -798,28 +798,28 @@
         <v>28</v>
       </c>
       <c r="C7">
-        <v>32205.06</v>
+        <v>35291.78</v>
       </c>
       <c r="D7">
-        <v>3121.32</v>
+        <v>3485.22</v>
       </c>
       <c r="E7">
-        <v>35326.38</v>
+        <v>38777</v>
       </c>
       <c r="F7">
-        <v>0.08051265000000005</v>
+        <v>0.08822945000000008</v>
       </c>
       <c r="G7">
-        <v>0.03121319999999997</v>
+        <v>0.03485219999999999</v>
       </c>
       <c r="H7">
-        <v>0.11172585</v>
+        <v>0.12308165</v>
       </c>
       <c r="I7">
-        <v>26.67749629493454</v>
+        <v>21.12230255438131</v>
       </c>
       <c r="J7">
-        <v>5.42</v>
+        <v>5.49</v>
       </c>
     </row>
   </sheetData>
@@ -875,28 +875,28 @@
         <v>26</v>
       </c>
       <c r="C2">
-        <v>6867617</v>
+        <v>6830425</v>
       </c>
       <c r="D2">
-        <v>815747</v>
+        <v>809495</v>
       </c>
       <c r="E2">
-        <v>7683364</v>
+        <v>7639920</v>
       </c>
       <c r="F2">
-        <v>17.16904250000003</v>
+        <v>17.07606250000003</v>
       </c>
       <c r="G2">
-        <v>8.157470000000032</v>
+        <v>8.094950000000029</v>
       </c>
       <c r="H2">
-        <v>25.32651249999999</v>
+        <v>25.17101249999999</v>
       </c>
       <c r="I2">
-        <v>42706.83864096203</v>
+        <v>45166.84336052323</v>
       </c>
       <c r="J2">
-        <v>19471</v>
+        <v>19336</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -907,28 +907,28 @@
         <v>27</v>
       </c>
       <c r="C3">
-        <v>5337899</v>
+        <v>5496563</v>
       </c>
       <c r="D3">
-        <v>619775</v>
+        <v>634498</v>
       </c>
       <c r="E3">
-        <v>5957674</v>
+        <v>6131061</v>
       </c>
       <c r="F3">
-        <v>13.34474750000001</v>
+        <v>13.74140750000001</v>
       </c>
       <c r="G3">
-        <v>6.197750000000013</v>
+        <v>6.344980000000014</v>
       </c>
       <c r="H3">
-        <v>19.54249749999998</v>
+        <v>20.08638749999999</v>
       </c>
       <c r="I3">
-        <v>32854.3018137482</v>
+        <v>34643.9341333895</v>
       </c>
       <c r="J3">
-        <v>15324</v>
+        <v>15760</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -939,28 +939,28 @@
         <v>28</v>
       </c>
       <c r="C4">
-        <v>3220506</v>
+        <v>3529178</v>
       </c>
       <c r="D4">
-        <v>312132</v>
+        <v>348522</v>
       </c>
       <c r="E4">
-        <v>3532638</v>
+        <v>3877700</v>
       </c>
       <c r="F4">
-        <v>8.051265000000004</v>
+        <v>8.822945000000008</v>
       </c>
       <c r="G4">
-        <v>3.121319999999997</v>
+        <v>3.485219999999999</v>
       </c>
       <c r="H4">
-        <v>11.172585</v>
+        <v>12.308165</v>
       </c>
       <c r="I4">
-        <v>20258.63611371885</v>
+        <v>19501.47495482466</v>
       </c>
       <c r="J4">
-        <v>9597</v>
+        <v>10437</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -971,25 +971,25 @@
         <v>26</v>
       </c>
       <c r="C5">
-        <v>6867617</v>
+        <v>6830425</v>
       </c>
       <c r="D5">
-        <v>815747</v>
+        <v>809495</v>
       </c>
       <c r="E5">
-        <v>7683364</v>
+        <v>7639920</v>
       </c>
       <c r="F5">
-        <v>17.16904250000003</v>
+        <v>17.07606250000003</v>
       </c>
       <c r="G5">
-        <v>8.157470000000032</v>
+        <v>8.094950000000029</v>
       </c>
       <c r="H5">
-        <v>25.32651249999999</v>
+        <v>25.17101249999999</v>
       </c>
       <c r="I5">
-        <v>3218.039707909571</v>
+        <v>2666.536554811988</v>
       </c>
       <c r="J5">
         <v>600</v>
@@ -1003,28 +1003,28 @@
         <v>27</v>
       </c>
       <c r="C6">
-        <v>5337899</v>
+        <v>5496563</v>
       </c>
       <c r="D6">
-        <v>619775</v>
+        <v>634498</v>
       </c>
       <c r="E6">
-        <v>5957674</v>
+        <v>6131061</v>
       </c>
       <c r="F6">
-        <v>13.34474750000001</v>
+        <v>13.74140750000001</v>
       </c>
       <c r="G6">
-        <v>6.197750000000013</v>
+        <v>6.344980000000014</v>
       </c>
       <c r="H6">
-        <v>19.54249749999998</v>
+        <v>20.08638749999999</v>
       </c>
       <c r="I6">
-        <v>3135.769980035722</v>
+        <v>2607.851395401056</v>
       </c>
       <c r="J6">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1035,28 +1035,28 @@
         <v>28</v>
       </c>
       <c r="C7">
-        <v>3220506</v>
+        <v>3529178</v>
       </c>
       <c r="D7">
-        <v>312132</v>
+        <v>348522</v>
       </c>
       <c r="E7">
-        <v>3532638</v>
+        <v>3877700</v>
       </c>
       <c r="F7">
-        <v>8.051265000000004</v>
+        <v>8.822945000000008</v>
       </c>
       <c r="G7">
-        <v>3.121319999999997</v>
+        <v>3.485219999999999</v>
       </c>
       <c r="H7">
-        <v>11.172585</v>
+        <v>12.308165</v>
       </c>
       <c r="I7">
-        <v>2667.749629493454</v>
+        <v>2112.230255438131</v>
       </c>
       <c r="J7">
-        <v>542</v>
+        <v>549</v>
       </c>
     </row>
   </sheetData>

</xml_diff>